<commit_message>
More work on ATR72_ATsi
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72 - ATsi/WEIGHTS/Weights.xlsx
+++ b/JPADSandBox_v2/out/ATR-72 - ATsi/WEIGHTS/Weights.xlsx
@@ -115,28 +115,28 @@
     <t>WEIGHT ESTIMATION METHODS COMPARISON</t>
   </si>
   <si>
+    <t>RAYMER</t>
+  </si>
+  <si>
+    <t>ROSKAM</t>
+  </si>
+  <si>
+    <t>NICOLAI_1984</t>
+  </si>
+  <si>
+    <t>KROO</t>
+  </si>
+  <si>
+    <t>TORENBEEK_1976</t>
+  </si>
+  <si>
+    <t>JENKINSON</t>
+  </si>
+  <si>
+    <t>SADRAEY</t>
+  </si>
+  <si>
     <t>TORENBEEK_2013</t>
-  </si>
-  <si>
-    <t>RAYMER</t>
-  </si>
-  <si>
-    <t>KROO</t>
-  </si>
-  <si>
-    <t>TORENBEEK_1976</t>
-  </si>
-  <si>
-    <t>ROSKAM</t>
-  </si>
-  <si>
-    <t>JENKINSON</t>
-  </si>
-  <si>
-    <t>SADRAEY</t>
-  </si>
-  <si>
-    <t>NICOLAI_1984</t>
   </si>
   <si>
     <t>TORENBEEK_1982</t>
@@ -611,10 +611,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>3698.0</v>
+        <v>3149.0</v>
       </c>
       <c r="D8" t="n">
-        <v>36.020643829108174</v>
+        <v>15.827205899908506</v>
       </c>
     </row>
     <row r="9">
@@ -625,10 +625,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>3149.0</v>
+        <v>3917.0</v>
       </c>
       <c r="D9" t="n">
-        <v>15.827205899908506</v>
+        <v>44.07594966971788</v>
       </c>
     </row>
     <row r="10">
@@ -639,10 +639,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>2585.0</v>
+        <v>2968.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-4.917965306045256</v>
+        <v>9.169624360409161</v>
       </c>
     </row>
     <row r="11">
@@ -653,10 +653,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>3818.0</v>
+        <v>2585.0</v>
       </c>
       <c r="D11" t="n">
-        <v>40.43451004314089</v>
+        <v>-4.917965306045256</v>
       </c>
     </row>
     <row r="12">
@@ -667,10 +667,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>3917.0</v>
+        <v>3818.0</v>
       </c>
       <c r="D12" t="n">
-        <v>44.07594966971788</v>
+        <v>40.43451004314089</v>
       </c>
     </row>
     <row r="13">
@@ -709,10 +709,10 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>2968.0</v>
+        <v>3698.0</v>
       </c>
       <c r="D15" t="n">
-        <v>9.169624360409161</v>
+        <v>36.020643829108174</v>
       </c>
     </row>
   </sheetData>
@@ -805,21 +805,21 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>2330.0</v>
+        <v>2613.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-19.148519821570545</v>
+        <v>-9.328361499469459</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -833,30 +833,30 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>2613.0</v>
+        <v>2539.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-9.328361499469459</v>
+        <v>-11.89617674977151</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>2539.0</v>
+        <v>2330.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-11.89617674977151</v>
+        <v>-19.148519821570545</v>
       </c>
     </row>
   </sheetData>
@@ -949,44 +949,44 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>144.0</v>
+        <v>207.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-53.9422655927021</v>
+        <v>-33.792006789509266</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>303.0</v>
+        <v>144.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-3.0868505179773305</v>
+        <v>-53.9422655927021</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>207.0</v>
+        <v>216.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-33.792006789509266</v>
+        <v>-30.91339838905315</v>
       </c>
     </row>
     <row r="11">
@@ -997,66 +997,66 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>236.0</v>
+        <v>303.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-24.516490832483992</v>
+        <v>-3.0868505179773305</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>124.0</v>
+        <v>236.0</v>
       </c>
       <c r="D12" t="n">
-        <v>-60.339173149271254</v>
+        <v>-24.516490832483992</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>216.0</v>
+        <v>293.0</v>
       </c>
       <c r="D13" t="n">
-        <v>-30.91339838905315</v>
+        <v>-6.285304296261907</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>293.0</v>
+        <v>273.0</v>
       </c>
       <c r="D14" t="n">
-        <v>-6.285304296261907</v>
+        <v>-12.68221185283106</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>273.0</v>
+        <v>124.0</v>
       </c>
       <c r="D15" t="n">
-        <v>-12.68221185283106</v>
+        <v>-60.339173149271254</v>
       </c>
     </row>
   </sheetData>
@@ -1149,44 +1149,44 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>89.0</v>
+        <v>445.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-71.53376137326727</v>
+        <v>42.33119313366365</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>256.0</v>
+        <v>89.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-18.11958327591484</v>
+        <v>-71.53376137326727</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>445.0</v>
+        <v>239.0</v>
       </c>
       <c r="D10" t="n">
-        <v>42.33119313366365</v>
+        <v>-23.55695469899862</v>
       </c>
     </row>
     <row r="11">
@@ -1197,10 +1197,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>338.0</v>
+        <v>256.0</v>
       </c>
       <c r="D11" t="n">
-        <v>8.107737706018687</v>
+        <v>-18.11958327591484</v>
       </c>
     </row>
     <row r="12">
@@ -1211,10 +1211,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>239.0</v>
+        <v>338.0</v>
       </c>
       <c r="D12" t="n">
-        <v>-23.55695469899862</v>
+        <v>8.107737706018687</v>
       </c>
     </row>
     <row r="13">
@@ -1359,7 +1359,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -1577,7 +1577,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -1777,7 +1777,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1793,7 +1793,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>

</xml_diff>